<commit_message>
today's simulations are done and added a spreadsheet for tracking computation time
</commit_message>
<xml_diff>
--- a/Simulation computation times.xlsx
+++ b/Simulation computation times.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ty/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ty/Box Sync/colliding ranges/Simulations_humans/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -44,10 +44,28 @@
     <t>Sim</t>
   </si>
   <si>
-    <t>Walltime (hours)</t>
-  </si>
-  <si>
     <t>Results</t>
+  </si>
+  <si>
+    <t>Walltime per core (hours)</t>
+  </si>
+  <si>
+    <t>calculation steps (tips * time)</t>
+  </si>
+  <si>
+    <t>Projected time to run (hours)</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>8-core Macpro</t>
+  </si>
+  <si>
+    <t>6-core Macpro</t>
+  </si>
+  <si>
+    <t>4.8 (ran as if 8 cores, so this number is misleading)</t>
   </si>
 </sst>
 </file>
@@ -83,9 +101,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,66 +384,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="25.5" customWidth="1"/>
+    <col min="7" max="7" width="43.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42571</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>300</v>
-      </c>
       <c r="D2">
         <v>300</v>
       </c>
       <c r="E2">
+        <v>300</v>
+      </c>
+      <c r="F2">
+        <f>D2*E2</f>
+        <v>90000</v>
+      </c>
+      <c r="G2" s="2">
         <v>3.57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42570</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>300</v>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
       <c r="D3">
         <v>300</v>
       </c>
       <c r="E3">
+        <v>300</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F24" si="0">D3*E3</f>
+        <v>90000</v>
+      </c>
+      <c r="G3" s="2">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>42571</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>300</v>
+      </c>
+      <c r="E4">
+        <v>300</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>90000</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>42572</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1200</v>
+      </c>
+      <c r="E5">
+        <v>300</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>360000</v>
+      </c>
+      <c r="H5" s="2">
+        <f>(F5/F2) *G$2</f>
+        <v>14.28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>42572</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1200</v>
+      </c>
+      <c r="E6">
+        <v>300</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>360000</v>
+      </c>
+      <c r="H6" s="2">
+        <f>(F6/F3) *G2</f>
+        <v>14.28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
confirming that I've pushed all new changes
</commit_message>
<xml_diff>
--- a/Simulation computation times.xlsx
+++ b/Simulation computation times.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>4.8 (ran as if 8 cores, so this number is misleading)</t>
+  </si>
+  <si>
+    <t>Start time</t>
+  </si>
+  <si>
+    <t>Projected end time</t>
   </si>
 </sst>
 </file>
@@ -101,12 +107,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -397,7 +404,7 @@
     <col min="8" max="8" width="25" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,8 +429,14 @@
       <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42571</v>
       </c>
@@ -447,7 +460,7 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42570</v>
       </c>
@@ -471,7 +484,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42571</v>
       </c>
@@ -495,7 +508,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>42572</v>
       </c>
@@ -517,8 +530,15 @@
         <f>(F5/F2) *G$2</f>
         <v>14.28</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="3">
+        <v>0.6479166666666667</v>
+      </c>
+      <c r="J5" s="3">
+        <f>I5+(H5 * 1/24)</f>
+        <v>1.2429166666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>42572</v>
       </c>
@@ -540,62 +560,69 @@
         <f>(F6/F3) *G2</f>
         <v>14.28</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="3">
+        <v>0.6479166666666667</v>
+      </c>
+      <c r="J6" s="3">
+        <f>I6+(H6 * 1/24)</f>
+        <v>1.2429166666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
new results for combo 25
</commit_message>
<xml_diff>
--- a/Simulation computation times.xlsx
+++ b/Simulation computation times.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Projected end time</t>
+  </si>
+  <si>
+    <t>model</t>
   </si>
 </sst>
 </file>
@@ -391,20 +394,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="25.5" customWidth="1"/>
-    <col min="7" max="7" width="43.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="43.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,28 +418,31 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42571</v>
       </c>
@@ -446,21 +452,21 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
-        <v>300</v>
-      </c>
       <c r="E2">
         <v>300</v>
       </c>
       <c r="F2">
-        <f>D2*E2</f>
+        <v>300</v>
+      </c>
+      <c r="G2">
+        <f>E2*F2</f>
         <v>90000</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>3.57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42570</v>
       </c>
@@ -470,21 +476,21 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>300</v>
-      </c>
       <c r="E3">
         <v>300</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F24" si="0">D3*E3</f>
+        <v>300</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G24" si="0">E3*F3</f>
         <v>90000</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42571</v>
       </c>
@@ -494,184 +500,329 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>300</v>
-      </c>
       <c r="E4">
         <v>300</v>
       </c>
       <c r="F4">
+        <v>300</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>90000</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>42572</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5">
+        <v>25</v>
+      </c>
+      <c r="E5">
         <v>1200</v>
       </c>
-      <c r="E5">
-        <v>300</v>
-      </c>
       <c r="F5">
+        <v>300</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>360000</v>
       </c>
       <c r="H5" s="2">
-        <f>(F5/F2) *G$2</f>
-        <v>14.28</v>
-      </c>
-      <c r="I5" s="3">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3">
         <v>0.6479166666666667</v>
       </c>
-      <c r="J5" s="3">
-        <f>I5+(H5 * 1/24)</f>
-        <v>1.2429166666666667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="3">
+        <f>J5+(I5 * 1/24)</f>
+        <v>1.0645833333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>42572</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6">
+        <v>28</v>
+      </c>
+      <c r="E6">
         <v>1200</v>
       </c>
-      <c r="E6">
-        <v>300</v>
-      </c>
       <c r="F6">
+        <v>300</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>360000</v>
       </c>
-      <c r="H6" s="2">
-        <f>(F6/F3) *G2</f>
+      <c r="I6" s="2">
+        <f>(G6/G3) *H2</f>
         <v>14.28</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
+        <f>K5</f>
+        <v>1.0645833333333334</v>
+      </c>
+      <c r="K6" s="3">
+        <f>J6+(I6 * 1/24)</f>
+        <v>1.6595833333333334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>42573</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>1200</v>
+      </c>
+      <c r="F7">
+        <v>300</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>42573</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <v>1200</v>
+      </c>
+      <c r="F8">
+        <v>300</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>42572</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>1200</v>
+      </c>
+      <c r="F9">
+        <v>300</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>360000</v>
+      </c>
+      <c r="H9" s="2">
+        <v>12</v>
+      </c>
+      <c r="I9" s="2">
+        <v>10</v>
+      </c>
+      <c r="J9" s="3">
         <v>0.6479166666666667</v>
       </c>
-      <c r="J6" s="3">
-        <f>I6+(H6 * 1/24)</f>
-        <v>1.2429166666666667</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="3">
+        <f>J9+(I9 * 1/24)</f>
+        <v>1.0645833333333334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>42572</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>28</v>
+      </c>
+      <c r="E10">
+        <v>1200</v>
+      </c>
       <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>360000</v>
+      </c>
+      <c r="I10" s="2">
+        <v>14.28</v>
+      </c>
+      <c r="J10" s="3">
+        <f>K9</f>
+        <v>1.0645833333333334</v>
+      </c>
+      <c r="K10" s="3">
+        <f>J10+(I10 * 1/24)</f>
+        <v>1.6595833333333334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>42573</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>1200</v>
+      </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>42573</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>31</v>
+      </c>
+      <c r="E12">
+        <v>1200</v>
+      </c>
       <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24">
+        <v>300</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
combo 28 results 1254 tips and 300 time steps
</commit_message>
<xml_diff>
--- a/Simulation computation times.xlsx
+++ b/Simulation computation times.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -574,6 +574,9 @@
         <f t="shared" si="0"/>
         <v>360000</v>
       </c>
+      <c r="H6" s="2">
+        <v>10</v>
+      </c>
       <c r="I6" s="2">
         <f>(G6/G3) *H2</f>
         <v>14.28</v>
@@ -694,6 +697,9 @@
       <c r="G10">
         <f t="shared" si="0"/>
         <v>360000</v>
+      </c>
+      <c r="H10" s="2">
+        <v>11</v>
       </c>
       <c r="I10" s="2">
         <v>14.28</v>

</xml_diff>

<commit_message>
end of this simulation run
</commit_message>
<xml_diff>
--- a/Simulation computation times.xlsx
+++ b/Simulation computation times.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>model</t>
+  </si>
+  <si>
+    <t>end time</t>
+  </si>
+  <si>
+    <t>total = 2.5 days</t>
+  </si>
+  <si>
+    <t>total = 2.3 days</t>
   </si>
 </sst>
 </file>
@@ -394,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -407,7 +416,7 @@
     <col min="9" max="9" width="25" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,8 +450,11 @@
       <c r="K1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42571</v>
       </c>
@@ -466,7 +478,7 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42570</v>
       </c>
@@ -490,7 +502,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42571</v>
       </c>
@@ -514,7 +526,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>42572</v>
       </c>
@@ -551,7 +563,7 @@
         <v>1.0645833333333334</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>42572</v>
       </c>
@@ -575,7 +587,7 @@
         <v>360000</v>
       </c>
       <c r="H6" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I6" s="2">
         <f>(G6/G3) *H2</f>
@@ -590,7 +602,7 @@
         <v>1.6595833333333334</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>42573</v>
       </c>
@@ -613,8 +625,14 @@
         <f t="shared" si="0"/>
         <v>360000</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H7" s="2">
+        <v>13</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.65902777777777777</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>42573</v>
       </c>
@@ -637,8 +655,14 @@
         <f t="shared" si="0"/>
         <v>360000</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.20069444444444443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>42572</v>
       </c>
@@ -675,7 +699,7 @@
         <v>1.0645833333333334</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>42572</v>
       </c>
@@ -699,7 +723,7 @@
         <v>360000</v>
       </c>
       <c r="H10" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I10" s="2">
         <v>14.28</v>
@@ -713,7 +737,7 @@
         <v>1.6595833333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>42573</v>
       </c>
@@ -736,8 +760,14 @@
         <f t="shared" si="0"/>
         <v>360000</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H11" s="2">
+        <v>15</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1.6595833333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>42573</v>
       </c>
@@ -760,26 +790,74 @@
         <f t="shared" si="0"/>
         <v>360000</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H12" s="2">
+        <v>18</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.35972222222222222</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.35972222222222222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>1200</v>
+      </c>
+      <c r="F13">
+        <v>1200</v>
+      </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1440000</v>
+      </c>
+      <c r="H13" s="2">
+        <f>SUM(H9:H12)</f>
+        <v>58</v>
+      </c>
+      <c r="I13" s="2">
+        <f>(G13*H13)/G12</f>
+        <v>232</v>
+      </c>
+      <c r="J13">
+        <f>I13/24</f>
+        <v>9.6666666666666661</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>1200</v>
+      </c>
+      <c r="F14">
+        <v>4800</v>
+      </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>5760000</v>
+      </c>
+      <c r="H14" s="2">
+        <f>SUM(H10:H13)</f>
+        <v>104</v>
+      </c>
+      <c r="I14" s="2">
+        <f>(G14*H14)/G13</f>
+        <v>416</v>
+      </c>
+      <c r="J14">
+        <f>I14/24</f>
+        <v>17.333333333333332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G16">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>